<commit_message>
update schedule and hw
</commit_message>
<xml_diff>
--- a/docs/data/schedule.xlsx
+++ b/docs/data/schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuarosenberg/s21-intro-to-data-sci-methods-in-ed/libs/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuarosenberg/s21-intro-to-data-sci-methods-in-ed/docs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF276568-6DDB-F244-A105-6339DDA5004C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D651A3D-E9F6-974D-8085-0EC7AB970104}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{3759121A-71D8-DD43-A2AE-D807B9ADF3B0}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,7 +637,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
@@ -651,7 +651,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
@@ -665,7 +665,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>23</v>
@@ -676,7 +676,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>26</v>

</xml_diff>